<commit_message>
An update with some findings
I have tried to do some "Fractaling" (creating chunks out of objects) no
success so far... Update on the time record
</commit_message>
<xml_diff>
--- a/Documentation/TimeRecord.xlsx
+++ b/Documentation/TimeRecord.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Item Woked On</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Building Back Together</t>
+  </si>
+  <si>
+    <t>NA YET</t>
   </si>
 </sst>
 </file>
@@ -385,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,7 +403,7 @@
     <col min="6" max="6" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,7 +420,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E2" s="1">
         <v>41287</v>
       </c>
@@ -425,7 +428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -442,7 +445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -459,13 +462,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
         <v>8</v>
       </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
       <c r="E5" s="1">
         <v>41290</v>
       </c>
@@ -473,13 +479,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
         <v>16</v>
       </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
       <c r="E6" s="1">
         <v>41291</v>
       </c>
@@ -487,7 +496,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -501,15 +510,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E8" s="1">
         <v>41293</v>
       </c>
       <c r="F8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <f>SUM(F2:F8)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E9" s="1">
         <v>41294</v>
       </c>
@@ -517,37 +530,59 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E10" s="1">
         <v>41295</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E11" s="1">
         <v>41296</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E12" s="1">
         <v>41297</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E13" s="1">
         <v>41298</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E14" s="1">
         <v>41299</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E15" s="1">
         <v>41300</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <f>SUM(F9:F15)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E16" s="1">
         <v>41301</v>
       </c>

</xml_diff>